<commit_message>
bug addon 0.1 new constants to neekeri2 botti
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\PythonCalc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nspire2\discord-bot-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40CCD69A-9F92-4DF0-8123-2BD414BBEE7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EFB68696-6EAE-4F65-B875-D4041CDF674C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="4155" windowWidth="21525" windowHeight="15660"/>
+    <workbookView xWindow="4392" yWindow="4152" windowWidth="21528" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>LaTeX</t>
   </si>
@@ -31,49 +31,100 @@
     <t>Description/Name</t>
   </si>
   <si>
-    <t>c_\\mathit{m}</t>
-  </si>
-  <si>
-    <t>Meter</t>
-  </si>
-  <si>
-    <t>c_\\mathit{s}</t>
-  </si>
-  <si>
     <t>Second</t>
   </si>
   <si>
-    <t>c_\\mathit{c}</t>
-  </si>
-  <si>
     <t>(299792458 \cdot \frac{c_\mathit{m}}{c_\mathit{s}})</t>
   </si>
   <si>
     <t>Lspeed</t>
   </si>
   <si>
-    <t>c_\\mathit{L}</t>
-  </si>
-  <si>
     <t>(1.616255 \cdot 10^{-35} \cdot c_\mathit{m})</t>
   </si>
   <si>
     <t>Planck length</t>
   </si>
   <si>
-    <t>c_\\mathit{h}</t>
-  </si>
-  <si>
     <t>(1.055 \cdot 10^{-34} \cdot c_\mathit{J} \dot c_\mathit{s})</t>
   </si>
   <si>
     <t>Planck constant</t>
+  </si>
+  <si>
+    <t>c_\mathit{J}</t>
+  </si>
+  <si>
+    <t>Joule</t>
+  </si>
+  <si>
+    <t>c_\mathit{c}</t>
+  </si>
+  <si>
+    <t>c_\mathit{L}</t>
+  </si>
+  <si>
+    <t>c_\mathit{h}</t>
+  </si>
+  <si>
+    <t>c_\mathit{s}</t>
+  </si>
+  <si>
+    <t>c_\mathit{m}</t>
+  </si>
+  <si>
+    <t>Metre</t>
+  </si>
+  <si>
+    <t>c_\mathit[K}</t>
+  </si>
+  <si>
+    <t>Kelvin</t>
+  </si>
+  <si>
+    <t>c_\mathit{rh}</t>
+  </si>
+  <si>
+    <t>\frac{\mathit{h}}{\mathit{2\cdot pi}}</t>
+  </si>
+  <si>
+    <t>Reduced Planck constant</t>
+  </si>
+  <si>
+    <t>Gravitational constant</t>
+  </si>
+  <si>
+    <t>c_\mathit{G}</t>
+  </si>
+  <si>
+    <t>c_\mathit{g]</t>
+  </si>
+  <si>
+    <t>Gramm</t>
+  </si>
+  <si>
+    <t>c_\mathit{N]</t>
+  </si>
+  <si>
+    <t>Newton</t>
+  </si>
+  <si>
+    <t>6.674\cdot10^{-11}\cdot\frac{N\cdotm^2}{kg^2}</t>
+  </si>
+  <si>
+    <t>c_\mathit{kg]</t>
+  </si>
+  <si>
+    <t>\mathit{g\cdot1000}</t>
+  </si>
+  <si>
+    <t>Kilogramm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -555,48 +606,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Aksentti1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Aksentti2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Aksentti3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Aksentti4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Aksentti5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Aksentti6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Huomautus" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Huono" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Hyvä" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Laskenta" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Linkitetty solu" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutraali" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Otsikko" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Otsikko 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Otsikko 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Otsikko 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Otsikko 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Selittävä teksti" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Summa" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Syöttö" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Tarkistussolu" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Tulostus" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Varoitusteksti" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -612,7 +663,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -907,19 +958,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,53 +983,118 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
neekeri-calculator bug addon 0.3 neekeri-calculator bug addon 0.3
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\PythonCalc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nspire2\cas-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4D076B-41C7-48D9-B281-BE5BD640A25B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EC6F609-5EF8-4204-B574-87CAA4329782}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="4020" windowWidth="21525" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3936" yWindow="4020" windowWidth="21528" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>LaTeX</t>
   </si>
@@ -119,6 +119,24 @@
   </si>
   <si>
     <t>(1.055 \cdot 10^{-34} \cdot c_\mathit{J} \cdot c_\mathit{s})</t>
+  </si>
+  <si>
+    <t>c_\mathit{pi}</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>3.14159265358979323846264338327950288419716939937510582097494459230781640628620899862803482534211706798214808651328230664709384460955058223172535940812848111745028410270193852110555964462294895493038196442881097566593344612847564823378678316527120190914564856692346034861045432664821339360726024914127372458700660631558817488152092096282925409171536436789259036001133053054882046652138414695194151160943305727036575959195309218611738193261179310511854807446237996274956735188575272489122793818301194912983367336244065664308602139494639522473719070217986094370277053921717629317675238467481846766940513200056812714526356082778577134275778960917363717872146844090122495343014654958537105079227968925892354201995611212902196086403441815981362977477130996051870721134999999837297804995105973173281609631859502445945534690830264252230825334468503526193118817101000313783875288658753320838142061717766914730359825349042875546873115956286388235378759375195778185778053217122680661300192787661119590921642019893809525720106548586327886593615338182796823030195203530185296899577362259941389124972177528347913151557485724245415069595082953311686172785588907509838175463746493931925506040092770167113900984882401285836160356370766010471018194295559619894676783744944825537977472684710404753464620804668425906949129331367702898915210475216205696602405803815019351125338243003558764024749647326391419927260426992279678235478163600934172164121992458631503028618297455570674983850549458858692699569092721079750930295532116534498720275596023648066549911988183479775356636980742654252786255181841757467289097777279380008164706001614524919217321721477235014144197356854816136115735255213347574184946843852332390739414333454776241686251898356948556209921922218427255025425688767179049460165346680498862723279178608578438382796797668145410095388378636095068006422512520511739298489608412848862694560424196528502221066118630674427862203919494504712371378696095636437191728746776465757396241389086583264599581339047802759009946576407895126946839835259570982582262052248940772671947826848260147699090264013639443745530506820349625245174939965143142980919065925093722169646151570985838741059788595977297549893016175392846813826868386894277415599185592524595395943104997252468084598727364469584865383673622262609912460805124388439045124413654976278079771569143599770012961608944169486855584840635342207222582848864815845602850601684273945226746767889525213852254995466672782398645659611635488623057745649803559363456817432411251507606947945109659609402522887971089314566913686722874894056010150330861792868092087476091782493858900971490967598526136554978189312978482168299894872265880485756401427047755513237964145152374623436454285844479526586782105114135473573952311342716610213596953623144295248493718711014576540359027993440374200731057853906219838744780847848968332144571386875194350643021845319104848100537061468067491927819119793995206141966342875444064374512371819217999839101591956181467514269123974894090718649423196156794520809514655022523160388193014209376213785595663893778708303906979207734672218256259966150142150306803844773454920260541466592520149744285073251866600213243408819071048633173464965145390579626856100550810665879699816357473638405257145910289706414011097120628043903975951567715770042033786993600723055876317635942187312514712053292819182618612586732157919841484882916447060957527069572209175671167229109816909152801735067127485832228718352093539657251210835791513698820914442100675103346711031412671113699086585163983150197016515116851714376576183515565088490998985998238734552833163550764791853589322618548963213293308985706420467525907091548</t>
+  </si>
+  <si>
+    <t>c_\mathtit{sm}</t>
+  </si>
+  <si>
+    <t>1.988435\cdot10^{30}\cdotkg</t>
+  </si>
+  <si>
+    <t>Mass of the sun</t>
   </si>
 </sst>
 </file>
@@ -606,48 +624,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Aksentti6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Aksentti6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Aksentti6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Aksentti1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Aksentti2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Aksentti3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Aksentti4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Aksentti5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Aksentti6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Huomautus" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Huono" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Hyvä" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Laskenta" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Linkitetty solu" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutraali" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Otsikko" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Otsikko 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Otsikko 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Otsikko 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Otsikko 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Selittävä teksti" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Summa" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Syöttö" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Tarkistussolu" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Tulostus" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Varoitusteksti" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -663,7 +681,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -959,20 +977,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -983,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -991,7 +1009,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1015,7 +1033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1023,7 +1041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1031,7 +1049,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1042,7 +1060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1053,7 +1071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1064,7 +1082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1075,7 +1093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1086,7 +1104,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1095,6 +1113,28 @@
       </c>
       <c r="C13" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>